<commit_message>
Logest Palindrome in string
</commit_message>
<xml_diff>
--- a/FINAL450 (1).xlsx
+++ b/FINAL450 (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\5th Sem\playlist 2\DSA_450_Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98100FE7-29D7-4D08-8CE2-FC39392735A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="474">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1420,33 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>Hints</t>
+  </si>
+  <si>
+    <t>Pointers start and end</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pointers start and end then match both pointers value</t>
+  </si>
+  <si>
+    <t>if more than one pointer point to string at that time if any single pointer change it value then other pointer value also be changed.</t>
+  </si>
+  <si>
+    <t>travers each letter form end of string and place this letter at start and check if new string matched rotated or not .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map first two string and then traversed suffled string and reduce map count </t>
+  </si>
+  <si>
+    <t>using recursion base case n==1 return "1" and then recursive call this call return a string store this string and using this string angai generate new string return new generated string</t>
+  </si>
+  <si>
+    <t>there could be even or odd palindrome hence traver first two pointers with zero gap which is even and other two pointer with one gap which is odd if both pointer's match then move left pointer left and right pointer to right and comapare while both matched after that store with these pointer's sub string.</t>
   </si>
 </sst>
 </file>
@@ -1855,30 +1876,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:C481"/>
+  <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="142.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:4" ht="24.6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="B2" s="10" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21">
+    <row r="4" spans="1:4" ht="21">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1888,13 +1910,19 @@
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="21">
+      <c r="D5" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="21">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1905,7 +1933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21">
+    <row r="7" spans="1:4" ht="21">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1916,7 +1944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21">
+    <row r="8" spans="1:4" ht="21">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1927,7 +1955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21">
+    <row r="9" spans="1:4" ht="21">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1938,7 +1966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21">
+    <row r="10" spans="1:4" ht="21">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1949,7 +1977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21">
+    <row r="11" spans="1:4" ht="21">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -1960,7 +1988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21">
+    <row r="12" spans="1:4" ht="21">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -1971,7 +1999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21">
+    <row r="13" spans="1:4" ht="21">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1982,7 +2010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21">
+    <row r="14" spans="1:4" ht="21">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -1993,7 +2021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21">
+    <row r="15" spans="1:4" ht="21">
       <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2004,7 +2032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21">
+    <row r="16" spans="1:4" ht="21">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -2358,7 +2386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="21">
+    <row r="49" spans="1:5" ht="21">
       <c r="A49" s="8" t="s">
         <v>42</v>
       </c>
@@ -2369,7 +2397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21">
+    <row r="50" spans="1:5" ht="21">
       <c r="A50" s="8" t="s">
         <v>42</v>
       </c>
@@ -2380,7 +2408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="21">
+    <row r="51" spans="1:5" ht="21">
       <c r="A51" s="8" t="s">
         <v>42</v>
       </c>
@@ -2391,7 +2419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21">
+    <row r="52" spans="1:5" ht="21">
       <c r="A52" s="8" t="s">
         <v>42</v>
       </c>
@@ -2402,7 +2430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="21">
+    <row r="53" spans="1:5" ht="21">
       <c r="A53" s="8" t="s">
         <v>42</v>
       </c>
@@ -2413,12 +2441,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="21">
+    <row r="55" spans="1:5" ht="21">
       <c r="A55" s="5"/>
       <c r="B55" s="7"/>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="21">
+    <row r="56" spans="1:5" ht="21">
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
@@ -2428,8 +2456,11 @@
       <c r="C56" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="21">
+      <c r="D56" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="21">
       <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
@@ -2439,8 +2470,14 @@
       <c r="C57" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="21">
+      <c r="D57" t="s">
+        <v>468</v>
+      </c>
+      <c r="E57" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="21">
       <c r="A58" s="5" t="s">
         <v>53</v>
       </c>
@@ -2450,8 +2487,11 @@
       <c r="C58" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="21">
+      <c r="D58" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="21">
       <c r="A59" s="5" t="s">
         <v>53</v>
       </c>
@@ -2462,7 +2502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="21">
+    <row r="60" spans="1:5" ht="21">
       <c r="A60" s="5" t="s">
         <v>53</v>
       </c>
@@ -2472,8 +2512,11 @@
       <c r="C60" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="21">
+      <c r="D60" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="21">
       <c r="A61" s="5" t="s">
         <v>53</v>
       </c>
@@ -2483,8 +2526,11 @@
       <c r="C61" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="21">
+      <c r="D61" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="21">
       <c r="A62" s="5" t="s">
         <v>53</v>
       </c>
@@ -2494,8 +2540,11 @@
       <c r="C62" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="21">
+      <c r="D62" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="21">
       <c r="A63" s="5" t="s">
         <v>53</v>
       </c>
@@ -2505,8 +2554,11 @@
       <c r="C63" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="21">
+      <c r="D63" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="21">
       <c r="A64" s="5" t="s">
         <v>53</v>
       </c>

</xml_diff>